<commit_message>
fix: pequeño movimiento pen_act
</commit_message>
<xml_diff>
--- a/res/egresos.xlsx
+++ b/res/egresos.xlsx
@@ -389,16 +389,16 @@
         <v>2025</v>
       </c>
       <c r="B2">
-        <v>1875064470.324741</v>
+        <v>1880467976.676862</v>
       </c>
       <c r="C2">
         <v>147956668.6968583</v>
       </c>
       <c r="D2">
-        <v>143264111.5775529</v>
+        <v>143665929.4907542</v>
       </c>
       <c r="E2">
-        <v>2166285250.599152</v>
+        <v>2172090574.864474</v>
       </c>
     </row>
     <row r="3">
@@ -406,16 +406,16 @@
         <v>2026</v>
       </c>
       <c r="B3">
-        <v>1764732611.347979</v>
+        <v>1775152818.585848</v>
       </c>
       <c r="C3">
         <v>273066058.2306628</v>
       </c>
       <c r="D3">
-        <v>145388875.9764523</v>
+        <v>146163748.0048345</v>
       </c>
       <c r="E3">
-        <v>2183187545.555094</v>
+        <v>2194382624.821345</v>
       </c>
     </row>
     <row r="4">
@@ -423,16 +423,16 @@
         <v>2027</v>
       </c>
       <c r="B4">
-        <v>1656591368.474839</v>
+        <v>1671639263.896055</v>
       </c>
       <c r="C4">
         <v>438296516.2419707</v>
       </c>
       <c r="D4">
-        <v>150803294.2675109</v>
+        <v>151922292.4775989</v>
       </c>
       <c r="E4">
-        <v>2245691178.984321</v>
+        <v>2261858072.615625</v>
       </c>
     </row>
     <row r="5">
@@ -440,16 +440,16 @@
         <v>2028</v>
       </c>
       <c r="B5">
-        <v>1554963587.057434</v>
+        <v>1574363313.820049</v>
       </c>
       <c r="C5">
         <v>683525971.3571392</v>
       </c>
       <c r="D5">
-        <v>162964223.8375448</v>
+        <v>164406834.8416693</v>
       </c>
       <c r="E5">
-        <v>2401453782.252118</v>
+        <v>2422296120.018857</v>
       </c>
     </row>
     <row r="6">
@@ -457,16 +457,16 @@
         <v>2029</v>
       </c>
       <c r="B6">
-        <v>1462868885.217533</v>
+        <v>1486252351.953044</v>
       </c>
       <c r="C6">
         <v>1010807382.464447</v>
       </c>
       <c r="D6">
-        <v>182258976.0562156</v>
+        <v>183997827.6823239</v>
       </c>
       <c r="E6">
-        <v>2655935243.738196</v>
+        <v>2681057562.099815</v>
       </c>
     </row>
     <row r="7">
@@ -474,16 +474,16 @@
         <v>2030</v>
       </c>
       <c r="B7">
-        <v>1369160247.033267</v>
+        <v>1396109940.869693</v>
       </c>
       <c r="C7">
         <v>1279070370.548541</v>
       </c>
       <c r="D7">
-        <v>196773669.2497726</v>
+        <v>198777714.2222583</v>
       </c>
       <c r="E7">
-        <v>2845004286.831581</v>
+        <v>2873958025.640492</v>
       </c>
     </row>
     <row r="8">
@@ -491,16 +491,16 @@
         <v>2031</v>
       </c>
       <c r="B8">
-        <v>1282903565.055856</v>
+        <v>1313158516.970951</v>
       </c>
       <c r="C8">
         <v>1521114122.510933</v>
       </c>
       <c r="D8">
-        <v>209761045.5679261</v>
+        <v>212010877.5937093</v>
       </c>
       <c r="E8">
-        <v>3013778733.134715</v>
+        <v>3046283517.075593</v>
       </c>
     </row>
     <row r="9">
@@ -508,16 +508,16 @@
         <v>2032</v>
       </c>
       <c r="B9">
-        <v>1199594784.064779</v>
+        <v>1232941557.194804</v>
       </c>
       <c r="C9">
         <v>1931554733.173261</v>
       </c>
       <c r="D9">
-        <v>236181515.6440885</v>
+        <v>238661263.0373417</v>
       </c>
       <c r="E9">
-        <v>3367331032.882129</v>
+        <v>3403157553.405407</v>
       </c>
     </row>
     <row r="10">
@@ -525,16 +525,16 @@
         <v>2033</v>
       </c>
       <c r="B10">
-        <v>1117146585.349733</v>
+        <v>1153082999.692729</v>
       </c>
       <c r="C10">
         <v>2205242037.287127</v>
       </c>
       <c r="D10">
-        <v>251900260.3990269</v>
+        <v>254572579.8298289</v>
       </c>
       <c r="E10">
-        <v>3574288883.035887</v>
+        <v>3612897616.809685</v>
       </c>
     </row>
     <row r="11">
@@ -542,16 +542,16 @@
         <v>2034</v>
       </c>
       <c r="B11">
-        <v>1047352320.78507</v>
+        <v>1085736210.798929</v>
       </c>
       <c r="C11">
         <v>2512930025.22141</v>
       </c>
       <c r="D11">
-        <v>271214261.6514485</v>
+        <v>274068581.3433015</v>
       </c>
       <c r="E11">
-        <v>3831496607.657928</v>
+        <v>3872734817.363641</v>
       </c>
     </row>
     <row r="12">
@@ -559,16 +559,16 @@
         <v>2035</v>
       </c>
       <c r="B12">
-        <v>975111042.196655</v>
+        <v>1015662966.074368</v>
       </c>
       <c r="C12">
         <v>2836802489.194846</v>
       </c>
       <c r="D12">
-        <v>291601209.0346817</v>
+        <v>294616749.0131697</v>
       </c>
       <c r="E12">
-        <v>4103514740.426182</v>
+        <v>4147082204.282383</v>
       </c>
     </row>
     <row r="13">
@@ -576,16 +576,16 @@
         <v>2036</v>
       </c>
       <c r="B13">
-        <v>908610399.5143454</v>
+        <v>950995473.6352975</v>
       </c>
       <c r="C13">
         <v>3153691234.761644</v>
       </c>
       <c r="D13">
-        <v>311849976.1159528</v>
+        <v>315001833.6181601</v>
       </c>
       <c r="E13">
-        <v>4374151610.391942</v>
+        <v>4419688542.015101</v>
       </c>
     </row>
     <row r="14">
@@ -593,16 +593,16 @@
         <v>2037</v>
       </c>
       <c r="B14">
-        <v>846465984.1270934</v>
+        <v>890378400.9906313</v>
       </c>
       <c r="C14">
         <v>3463674136.821453</v>
       </c>
       <c r="D14">
-        <v>331864542.1494482</v>
+        <v>335129976.5836653</v>
       </c>
       <c r="E14">
-        <v>4642004663.097995</v>
+        <v>4689182514.395749</v>
       </c>
     </row>
     <row r="15">
@@ -610,16 +610,16 @@
         <v>2038</v>
       </c>
       <c r="B15">
-        <v>786784130.4657413</v>
+        <v>831918878.253419</v>
       </c>
       <c r="C15">
         <v>3769626800.819961</v>
       </c>
       <c r="D15">
-        <v>351730563.8435864</v>
+        <v>355086893.7869734</v>
       </c>
       <c r="E15">
-        <v>4908141495.129288</v>
+        <v>4956632572.860353</v>
       </c>
     </row>
     <row r="16">
@@ -627,16 +627,16 @@
         <v>2039</v>
       </c>
       <c r="B16">
-        <v>732096322.3411342</v>
+        <v>778122743.8835673</v>
       </c>
       <c r="C16">
         <v>4033448711.492968</v>
       </c>
       <c r="D16">
-        <v>368642938.1500763</v>
+        <v>372065575.1289406</v>
       </c>
       <c r="E16">
-        <v>5134187971.984178</v>
+        <v>5183637030.505476</v>
       </c>
     </row>
     <row r="17">
@@ -644,16 +644,16 @@
         <v>2040</v>
       </c>
       <c r="B17">
-        <v>679417834.4838989</v>
+        <v>725987916.2432363</v>
       </c>
       <c r="C17">
         <v>4404170965.036217</v>
       </c>
       <c r="D17">
-        <v>394091983.8182482</v>
+        <v>397555048.6970003</v>
       </c>
       <c r="E17">
-        <v>5477680783.338364</v>
+        <v>5527713929.976454</v>
       </c>
     </row>
     <row r="18">
@@ -661,16 +661,16 @@
         <v>2041</v>
       </c>
       <c r="B18">
-        <v>629113315.0797588</v>
+        <v>675909485.5478243</v>
       </c>
       <c r="C18">
         <v>4667115574.873791</v>
       </c>
       <c r="D18">
-        <v>411234458.9860638</v>
+        <v>414714336.3726987</v>
       </c>
       <c r="E18">
-        <v>5707463348.939613</v>
+        <v>5757739396.794313</v>
       </c>
     </row>
     <row r="19">
@@ -678,16 +678,16 @@
         <v>2042</v>
       </c>
       <c r="B19">
-        <v>580912503.963037</v>
+        <v>627617933.7428812</v>
       </c>
       <c r="C19">
         <v>4891544067.564852</v>
       </c>
       <c r="D19">
-        <v>425493793.2958391</v>
+        <v>428966922.9835526</v>
       </c>
       <c r="E19">
-        <v>5897950364.823729</v>
+        <v>5948128924.291286</v>
       </c>
     </row>
     <row r="20">
@@ -695,16 +695,16 @@
         <v>2043</v>
       </c>
       <c r="B20">
-        <v>535339939.974487</v>
+        <v>581585248.030279</v>
       </c>
       <c r="C20">
         <v>5143192292.533134</v>
       </c>
       <c r="D20">
-        <v>442075309.4874511</v>
+        <v>445514223.401382</v>
       </c>
       <c r="E20">
-        <v>6120607541.995072</v>
+        <v>6170291763.964795</v>
       </c>
     </row>
     <row r="21">
@@ -712,16 +712,16 @@
         <v>2044</v>
       </c>
       <c r="B21">
-        <v>491784441.3606832</v>
+        <v>537284885.8940061</v>
       </c>
       <c r="C21">
         <v>5495846568.552362</v>
       </c>
       <c r="D21">
-        <v>466732517.545981</v>
+        <v>470116041.5914239</v>
       </c>
       <c r="E21">
-        <v>6454363527.459027</v>
+        <v>6503247496.037792</v>
       </c>
     </row>
     <row r="22">
@@ -729,16 +729,16 @@
         <v>2045</v>
       </c>
       <c r="B22">
-        <v>450213033.3086699</v>
+        <v>494651983.2494506</v>
       </c>
       <c r="C22">
         <v>5820090731.117184</v>
       </c>
       <c r="D22">
-        <v>489293007.2327493</v>
+        <v>492597595.9509704</v>
       </c>
       <c r="E22">
-        <v>6759596771.658603</v>
+        <v>6807340310.317605</v>
       </c>
     </row>
     <row r="23">
@@ -746,16 +746,16 @@
         <v>2046</v>
       </c>
       <c r="B23">
-        <v>410613700.7039741</v>
+        <v>453684530.2832677</v>
       </c>
       <c r="C23">
         <v>6089648915.16651</v>
       </c>
       <c r="D23">
-        <v>507691168.7054584</v>
+        <v>510894020.656322</v>
       </c>
       <c r="E23">
-        <v>7007953784.575942</v>
+        <v>7054227466.1061</v>
       </c>
     </row>
     <row r="24">
@@ -763,16 +763,16 @@
         <v>2047</v>
       </c>
       <c r="B24">
-        <v>372959422.5602459</v>
+        <v>414381308.2901382</v>
       </c>
       <c r="C24">
         <v>6318139849.300166</v>
       </c>
       <c r="D24">
-        <v>522995541.9256024</v>
+        <v>526075774.38953</v>
       </c>
       <c r="E24">
-        <v>7214094813.786014</v>
+        <v>7258596931.979835</v>
       </c>
     </row>
     <row r="25">
@@ -780,16 +780,16 @@
         <v>2048</v>
       </c>
       <c r="B25">
-        <v>337215274.1898295</v>
+        <v>376724769.7368712</v>
       </c>
       <c r="C25">
         <v>6521743440.901905</v>
       </c>
       <c r="D25">
-        <v>536475407.3102698</v>
+        <v>539413429.7752774</v>
       </c>
       <c r="E25">
-        <v>7395434122.402004</v>
+        <v>7437881640.414054</v>
       </c>
     </row>
     <row r="26">
@@ -797,16 +797,16 @@
         <v>2049</v>
       </c>
       <c r="B26">
-        <v>303376935.7130885</v>
+        <v>340737916.9127936</v>
       </c>
       <c r="C26">
         <v>6582451142.033695</v>
       </c>
       <c r="D26">
-        <v>538856889.1206682</v>
+        <v>541635142.8179032</v>
       </c>
       <c r="E26">
-        <v>7424684966.867452</v>
+        <v>7464824201.764392</v>
       </c>
     </row>
     <row r="27">
@@ -814,16 +814,16 @@
         <v>2050</v>
       </c>
       <c r="B27">
-        <v>271452610.3505541</v>
+        <v>306461849.3207991</v>
       </c>
       <c r="C27">
         <v>6668801554.021118</v>
       </c>
       <c r="D27">
-        <v>543385720.8340713</v>
+        <v>545989093.2424821</v>
       </c>
       <c r="E27">
-        <v>7483639885.205744</v>
+        <v>7521252496.584399</v>
       </c>
     </row>
     <row r="28">
@@ -831,16 +831,16 @@
         <v>2051</v>
       </c>
       <c r="B28">
-        <v>241458065.2097805</v>
+        <v>273948733.211027</v>
       </c>
       <c r="C28">
         <v>6690687000.545776</v>
       </c>
       <c r="D28">
-        <v>542982147.6006281</v>
+        <v>545398232.9281948</v>
       </c>
       <c r="E28">
-        <v>7475127213.356185</v>
+        <v>7510033966.684999</v>
       </c>
     </row>
     <row r="29">
@@ -848,16 +848,16 @@
         <v>2052</v>
       </c>
       <c r="B29">
-        <v>213419229.5000036</v>
+        <v>243265697.9505706</v>
       </c>
       <c r="C29">
         <v>6663102818.674589</v>
       </c>
       <c r="D29">
-        <v>538826802.5889829</v>
+        <v>541046258.7879237</v>
       </c>
       <c r="E29">
-        <v>7415348850.763576</v>
+        <v>7447414775.413083</v>
       </c>
     </row>
     <row r="30">
@@ -865,16 +865,16 @@
         <v>2053</v>
       </c>
       <c r="B30">
-        <v>187356017.1478409</v>
+        <v>214478735.380334</v>
       </c>
       <c r="C30">
         <v>6540030476.5349</v>
       </c>
       <c r="D30">
-        <v>527305089.3150839</v>
+        <v>529322000.8037223</v>
       </c>
       <c r="E30">
-        <v>7254691582.997824</v>
+        <v>7283831212.718956</v>
       </c>
     </row>
     <row r="31">
@@ -882,16 +882,16 @@
         <v>2054</v>
       </c>
       <c r="B31">
-        <v>163284504.2168144</v>
+        <v>187652812.0972563</v>
       </c>
       <c r="C31">
         <v>6386691959.171655</v>
       </c>
       <c r="D31">
-        <v>513544171.895604</v>
+        <v>515356258.7115877</v>
       </c>
       <c r="E31">
-        <v>7063520635.284073</v>
+        <v>7089701029.980499</v>
       </c>
     </row>
     <row r="32">
@@ -899,16 +899,16 @@
         <v>2055</v>
       </c>
       <c r="B32">
-        <v>141224866.1825184</v>
+        <v>162858495.4033191</v>
       </c>
       <c r="C32">
         <v>6200995099.090839</v>
       </c>
       <c r="D32">
-        <v>497381526.0773829</v>
+        <v>498990255.5174913</v>
       </c>
       <c r="E32">
-        <v>6839601491.35074</v>
+        <v>6862843850.01165</v>
       </c>
     </row>
     <row r="33">
@@ -916,16 +916,16 @@
         <v>2056</v>
       </c>
       <c r="B33">
-        <v>121193652.3915122</v>
+        <v>140162378.3742007</v>
       </c>
       <c r="C33">
         <v>5963985960.599737</v>
       </c>
       <c r="D33">
-        <v>477329262.3797031</v>
+        <v>478739823.1144854</v>
       </c>
       <c r="E33">
-        <v>6562508875.370953</v>
+        <v>6582888162.088424</v>
       </c>
     </row>
     <row r="34">
@@ -933,16 +933,16 @@
         <v>2057</v>
       </c>
       <c r="B34">
-        <v>103179586.957252</v>
+        <v>119599554.345527</v>
       </c>
       <c r="C34">
         <v>5701901190.083423</v>
       </c>
       <c r="D34">
-        <v>455448873.071623</v>
+        <v>456669901.9000981</v>
       </c>
       <c r="E34">
-        <v>6260529650.112297</v>
+        <v>6278170646.329047</v>
       </c>
     </row>
     <row r="35">
@@ -950,16 +950,16 @@
         <v>2058</v>
       </c>
       <c r="B35">
-        <v>87146791.08947648</v>
+        <v>101175172.4034119</v>
       </c>
       <c r="C35">
         <v>5428627332.4453</v>
       </c>
       <c r="D35">
-        <v>432829518.4883719</v>
+        <v>433872703.1425258</v>
       </c>
       <c r="E35">
-        <v>5948603642.023149</v>
+        <v>5963675207.991238</v>
       </c>
     </row>
     <row r="36">
@@ -967,16 +967,16 @@
         <v>2059</v>
       </c>
       <c r="B36">
-        <v>73042001.80689466</v>
+        <v>84871191.67845982</v>
       </c>
       <c r="C36">
         <v>5156752872.568609</v>
       </c>
       <c r="D36">
-        <v>410457068.6496215</v>
+        <v>411336716.0635988</v>
       </c>
       <c r="E36">
-        <v>5640251943.025126</v>
+        <v>5652960780.310668</v>
       </c>
     </row>
     <row r="37">
@@ -984,16 +984,16 @@
         <v>2060</v>
       </c>
       <c r="B37">
-        <v>60787925.89934213</v>
+        <v>70636890.22847228</v>
       </c>
       <c r="C37">
         <v>4866878298.688068</v>
       </c>
       <c r="D37">
-        <v>386801809.3621863</v>
+        <v>387534202.3744329</v>
       </c>
       <c r="E37">
-        <v>5314468033.949597</v>
+        <v>5325049391.290974</v>
       </c>
     </row>
     <row r="38">
@@ -1001,16 +1001,16 @@
         <v>2061</v>
       </c>
       <c r="B38">
-        <v>50278812.43350112</v>
+        <v>58381900.22765249</v>
       </c>
       <c r="C38">
         <v>4575106060.840212</v>
       </c>
       <c r="D38">
-        <v>363121887.7898805</v>
+        <v>363724453.1642423</v>
       </c>
       <c r="E38">
-        <v>4988506761.063594</v>
+        <v>4997212414.232107</v>
       </c>
     </row>
     <row r="39">
@@ -1018,16 +1018,16 @@
         <v>2062</v>
       </c>
       <c r="B39">
-        <v>41382571.27354696</v>
+        <v>47978599.24389503</v>
       </c>
       <c r="C39">
         <v>4289646418.587631</v>
       </c>
       <c r="D39">
-        <v>340053274.5058427</v>
+        <v>340543771.2355118</v>
       </c>
       <c r="E39">
-        <v>4671082264.367022</v>
+        <v>4678168789.067038</v>
       </c>
     </row>
     <row r="40">
@@ -1035,16 +1035,16 @@
         <v>2063</v>
       </c>
       <c r="B40">
-        <v>33945194.73889415</v>
+        <v>39267920.6717283</v>
       </c>
       <c r="C40">
         <v>4009845592.741255</v>
       </c>
       <c r="D40">
-        <v>317533721.1967995</v>
+        <v>317929532.0809735</v>
       </c>
       <c r="E40">
-        <v>4361324508.676949</v>
+        <v>4367043045.493957</v>
       </c>
     </row>
     <row r="41">
@@ -1052,16 +1052,16 @@
         <v>2064</v>
       </c>
       <c r="B41">
-        <v>27794318.76196122</v>
+        <v>32062918.38513686</v>
       </c>
       <c r="C41">
         <v>3729979177.934872</v>
       </c>
       <c r="D41">
-        <v>295101133.9043307</v>
+        <v>295418557.3847718</v>
       </c>
       <c r="E41">
-        <v>4052874630.601163</v>
+        <v>4057460653.704781</v>
       </c>
     </row>
     <row r="42">
@@ -1069,16 +1069,16 @@
         <v>2065</v>
       </c>
       <c r="B42">
-        <v>22758324.69285481</v>
+        <v>26170788.96388649</v>
       </c>
       <c r="C42">
         <v>3455256974.278594</v>
       </c>
       <c r="D42">
-        <v>273152667.7426257</v>
+        <v>273406426.909897</v>
       </c>
       <c r="E42">
-        <v>3751167966.714075</v>
+        <v>3754834190.152377</v>
       </c>
     </row>
     <row r="43">
@@ -1086,16 +1086,16 @@
         <v>2066</v>
       </c>
       <c r="B43">
-        <v>18665328.68435691</v>
+        <v>21393716.56128882</v>
       </c>
       <c r="C43">
         <v>3197104658.60184</v>
       </c>
       <c r="D43">
-        <v>252573911.3028589</v>
+        <v>252776800.8807867</v>
       </c>
       <c r="E43">
-        <v>3468343898.589055</v>
+        <v>3471275176.043915</v>
       </c>
     </row>
     <row r="44">
@@ -1103,16 +1103,16 @@
         <v>2067</v>
       </c>
       <c r="B44">
-        <v>15351621.15241775</v>
+        <v>17539967.58056776</v>
       </c>
       <c r="C44">
         <v>2947974373.043943</v>
       </c>
       <c r="D44">
-        <v>232759956.9464609</v>
+        <v>232922687.7249258</v>
       </c>
       <c r="E44">
-        <v>3196085951.142821</v>
+        <v>3198437028.349437</v>
       </c>
     </row>
     <row r="45">
@@ -1120,16 +1120,16 @@
         <v>2068</v>
       </c>
       <c r="B45">
-        <v>12669520.57881755</v>
+        <v>14434607.1816467</v>
       </c>
       <c r="C45">
         <v>2707433167.672991</v>
       </c>
       <c r="D45">
-        <v>213666163.9305695</v>
+        <v>213797420.0759592</v>
       </c>
       <c r="E45">
-        <v>2933768852.182378</v>
+        <v>2935665194.930597</v>
       </c>
     </row>
     <row r="46">
@@ -1137,16 +1137,16 @@
         <v>2069</v>
       </c>
       <c r="B46">
-        <v>10492127.39267628</v>
+        <v>11926109.49335095</v>
       </c>
       <c r="C46">
         <v>2477144500.387847</v>
       </c>
       <c r="D46">
-        <v>195414131.1322827</v>
+        <v>195520765.5392238</v>
       </c>
       <c r="E46">
-        <v>2683050758.912806</v>
+        <v>2684591375.420422</v>
       </c>
     </row>
     <row r="47">
@@ -1154,16 +1154,16 @@
         <v>2070</v>
       </c>
       <c r="B47">
-        <v>8714773.495707419</v>
+        <v>9888793.784750223</v>
       </c>
       <c r="C47">
         <v>2259461632.950758</v>
       </c>
       <c r="D47">
-        <v>178181264.2508153</v>
+        <v>178268567.2633146</v>
       </c>
       <c r="E47">
-        <v>2446357670.697281</v>
+        <v>2447618993.998823</v>
       </c>
     </row>
     <row r="48">
@@ -1171,16 +1171,16 @@
         <v>2071</v>
       </c>
       <c r="B48">
-        <v>7253373.558158772</v>
+        <v>8221547.623054586</v>
       </c>
       <c r="C48">
         <v>2054287083.099996</v>
       </c>
       <c r="D48">
-        <v>161953858.4613672</v>
+        <v>162025854.246515</v>
       </c>
       <c r="E48">
-        <v>2223494315.119522</v>
+        <v>2224534484.969565</v>
       </c>
     </row>
     <row r="49">
@@ -1188,16 +1188,16 @@
         <v>2072</v>
       </c>
       <c r="B49">
-        <v>6042432.692949591</v>
+        <v>6845666.43053335</v>
       </c>
       <c r="C49">
         <v>1861205626.894347</v>
       </c>
       <c r="D49">
-        <v>146694584.3094311</v>
+        <v>146754314.7294984</v>
       </c>
       <c r="E49">
-        <v>2013942643.896728</v>
+        <v>2014805608.054379</v>
       </c>
     </row>
     <row r="50">
@@ -1205,16 +1205,16 @@
         <v>2073</v>
       </c>
       <c r="B50">
-        <v>5031742.409733593</v>
+        <v>5701040.522837179</v>
       </c>
       <c r="C50">
         <v>1679815637.094098</v>
       </c>
       <c r="D50">
-        <v>132368286.6421663</v>
+        <v>132418057.2824861</v>
       </c>
       <c r="E50">
-        <v>1817215666.145998</v>
+        <v>1817934734.899421</v>
       </c>
     </row>
     <row r="51">
@@ -1222,16 +1222,16 @@
         <v>2074</v>
       </c>
       <c r="B51">
-        <v>4183219.59936509</v>
+        <v>4742338.330414427</v>
       </c>
       <c r="C51">
         <v>1509803548.545943</v>
       </c>
       <c r="D51">
-        <v>118947605.9462698</v>
+        <v>118989183.3789776</v>
       </c>
       <c r="E51">
-        <v>1632934374.091578</v>
+        <v>1633535070.255335</v>
       </c>
     </row>
     <row r="52">
@@ -1239,16 +1239,16 @@
         <v>2075</v>
       </c>
       <c r="B52">
-        <v>3467929.091475662</v>
+        <v>3935312.034524159</v>
       </c>
       <c r="C52">
         <v>1350941625.273656</v>
       </c>
       <c r="D52">
-        <v>106412585.9843231</v>
+        <v>106447341.7200627</v>
       </c>
       <c r="E52">
-        <v>1460822140.349455</v>
+        <v>1461324279.028243</v>
       </c>
     </row>
     <row r="53">
@@ -1256,16 +1256,16 @@
         <v>2076</v>
       </c>
       <c r="B53">
-        <v>2863315.370010779</v>
+        <v>3253456.68472141</v>
       </c>
       <c r="C53">
         <v>1202966748.352674</v>
       </c>
       <c r="D53">
-        <v>94740947.87687455</v>
+        <v>94769959.73671423</v>
       </c>
       <c r="E53">
-        <v>1300571011.59956</v>
+        <v>1300990164.77411</v>
       </c>
     </row>
     <row r="54">
@@ -1273,16 +1273,16 @@
         <v>2077</v>
       </c>
       <c r="B54">
-        <v>2351411.686863653</v>
+        <v>2675864.364052457</v>
       </c>
       <c r="C54">
         <v>1065602028.686601</v>
       </c>
       <c r="D54">
-        <v>83909659.80409902</v>
+        <v>83933786.89661726</v>
       </c>
       <c r="E54">
-        <v>1151863100.177564</v>
+        <v>1152211679.947271</v>
       </c>
     </row>
     <row r="55">
@@ -1290,16 +1290,16 @@
         <v>2078</v>
       </c>
       <c r="B55">
-        <v>1917768.574611927</v>
+        <v>2185887.61838073</v>
       </c>
       <c r="C55">
         <v>938594769.8476171</v>
       </c>
       <c r="D55">
-        <v>73897842.71059029</v>
+        <v>73917780.69671191</v>
       </c>
       <c r="E55">
-        <v>1014410381.132819</v>
+        <v>1014698438.16271</v>
       </c>
     </row>
     <row r="56">
@@ -1307,16 +1307,16 @@
         <v>2079</v>
       </c>
       <c r="B56">
-        <v>1550848.761228028</v>
+        <v>1770392.4195152</v>
       </c>
       <c r="C56">
         <v>821747504.1524661</v>
       </c>
       <c r="D56">
-        <v>64689165.50739458</v>
+        <v>64705491.30936109</v>
       </c>
       <c r="E56">
-        <v>887987518.4210887</v>
+        <v>888223387.8813424</v>
       </c>
     </row>
     <row r="57">
@@ -1324,16 +1324,16 @@
         <v>2080</v>
       </c>
       <c r="B57">
-        <v>1241422.592155998</v>
+        <v>1419019.702575519</v>
       </c>
       <c r="C57">
         <v>714864325.9983813</v>
       </c>
       <c r="D57">
-        <v>56267583.96483537</v>
+        <v>56280790.51918157</v>
       </c>
       <c r="E57">
-        <v>772373332.5553727</v>
+        <v>772564136.2201384</v>
       </c>
     </row>
     <row r="58">
@@ -1341,16 +1341,16 @@
         <v>2081</v>
       </c>
       <c r="B58">
-        <v>981910.5932514627</v>
+        <v>1123389.916759512</v>
       </c>
       <c r="C58">
         <v>617690250.9905381</v>
       </c>
       <c r="D58">
-        <v>48612528.21692829</v>
+        <v>48623048.96453707</v>
       </c>
       <c r="E58">
-        <v>667284689.8007178</v>
+        <v>667436689.8718346</v>
       </c>
     </row>
     <row r="59">
@@ -1358,16 +1358,16 @@
         <v>2082</v>
       </c>
       <c r="B59">
-        <v>765986.9835814735</v>
+        <v>876625.3989582431</v>
       </c>
       <c r="C59">
         <v>529920945.8689792</v>
       </c>
       <c r="D59">
-        <v>41699639.49233224</v>
+        <v>41707866.83478168</v>
       </c>
       <c r="E59">
-        <v>572386572.3448929</v>
+        <v>572505438.1027191</v>
       </c>
     </row>
     <row r="60">
@@ -1375,16 +1375,16 @@
         <v>2083</v>
       </c>
       <c r="B60">
-        <v>588286.628901816</v>
+        <v>672963.9512070213</v>
       </c>
       <c r="C60">
         <v>451211201.7353225</v>
       </c>
       <c r="D60">
-        <v>35501414.96251971</v>
+        <v>35507711.77476104</v>
       </c>
       <c r="E60">
-        <v>487300903.326744</v>
+        <v>487391877.4612905</v>
       </c>
     </row>
     <row r="61">
@@ -1392,16 +1392,16 @@
         <v>2084</v>
       </c>
       <c r="B61">
-        <v>444106.9935460061</v>
+        <v>507361.5345739124</v>
       </c>
       <c r="C61">
         <v>381191203.6131744</v>
       </c>
       <c r="D61">
-        <v>29988464.62914506</v>
+        <v>29993168.39111368</v>
       </c>
       <c r="E61">
-        <v>411623775.2358655</v>
+        <v>411691733.538862</v>
       </c>
     </row>
     <row r="62">
@@ -1409,16 +1409,16 @@
         <v>2085</v>
       </c>
       <c r="B62">
-        <v>329133.9265294261</v>
+        <v>375146.4405565684</v>
       </c>
       <c r="C62">
         <v>319445939.3129843</v>
       </c>
       <c r="D62">
-        <v>25127873.18942212</v>
+        <v>25131294.79220422</v>
       </c>
       <c r="E62">
-        <v>344902946.4289358</v>
+        <v>344952380.5457451</v>
       </c>
     </row>
     <row r="63">
@@ -1426,16 +1426,16 @@
         <v>2086</v>
       </c>
       <c r="B63">
-        <v>239215.5511918278</v>
+        <v>271737.6517831757</v>
       </c>
       <c r="C63">
         <v>265481056.5849613</v>
       </c>
       <c r="D63">
-        <v>20880500.41582103</v>
+        <v>20882918.83855268</v>
       </c>
       <c r="E63">
-        <v>286600772.5519741</v>
+        <v>286635713.0752971</v>
       </c>
     </row>
     <row r="64">
@@ -1443,16 +1443,16 @@
         <v>2087</v>
       </c>
       <c r="B64">
-        <v>170338.3420552253</v>
+        <v>192623.7383773833</v>
       </c>
       <c r="C64">
         <v>218737412.4829796</v>
       </c>
       <c r="D64">
-        <v>17202122.83057161</v>
+        <v>17203780.02700324</v>
       </c>
       <c r="E64">
-        <v>236109873.6556065</v>
+        <v>236133816.2483602</v>
       </c>
     </row>
     <row r="65">
@@ -1460,16 +1460,16 @@
         <v>2088</v>
       </c>
       <c r="B65">
-        <v>118711.2550494728</v>
+        <v>133475.124965423</v>
       </c>
       <c r="C65">
         <v>178621698.4656633</v>
       </c>
       <c r="D65">
-        <v>14045846.47132421</v>
+        <v>14046944.3487049</v>
       </c>
       <c r="E65">
-        <v>192786256.1920369</v>
+        <v>192802117.9393336</v>
       </c>
     </row>
     <row r="66">
@@ -1477,16 +1477,16 @@
         <v>2089</v>
       </c>
       <c r="B66">
-        <v>80883.48817197191</v>
+        <v>90306.5224406873</v>
       </c>
       <c r="C66">
         <v>144531300.0536281</v>
       </c>
       <c r="D66">
-        <v>11364069.13206862</v>
+        <v>11364769.8518826</v>
       </c>
       <c r="E66">
-        <v>155976252.6738687</v>
+        <v>155986376.4279514</v>
       </c>
     </row>
     <row r="67">
@@ -1494,16 +1494,16 @@
         <v>2090</v>
       </c>
       <c r="B67">
-        <v>53813.39291971231</v>
+        <v>59579.33168091041</v>
       </c>
       <c r="C67">
         <v>115854981.571022</v>
       </c>
       <c r="D67">
-        <v>9108539.30590136</v>
+        <v>9108968.075172588</v>
       </c>
       <c r="E67">
-        <v>125017334.2698431</v>
+        <v>125023528.9778755</v>
       </c>
     </row>
     <row r="68">
@@ -1511,16 +1511,16 @@
         <v>2091</v>
       </c>
       <c r="B68">
-        <v>34905.00498658049</v>
+        <v>38262.16988631983</v>
       </c>
       <c r="C68">
         <v>91975629.30186424</v>
       </c>
       <c r="D68">
-        <v>7230574.657074297</v>
+        <v>7230824.304045427</v>
       </c>
       <c r="E68">
-        <v>99241108.96392512</v>
+        <v>99244715.77579598</v>
       </c>
     </row>
     <row r="69">
@@ -1528,16 +1528,16 @@
         <v>2092</v>
       </c>
       <c r="B69">
-        <v>22034.1725601988</v>
+        <v>23875.58012389936</v>
       </c>
       <c r="C69">
         <v>72289011.787893</v>
       </c>
       <c r="D69">
-        <v>5682538.520303669</v>
+        <v>5682675.451861881</v>
       </c>
       <c r="E69">
-        <v>77993584.48075686</v>
+        <v>77995562.81987879</v>
       </c>
     </row>
     <row r="70">
@@ -1545,16 +1545,16 @@
         <v>2093</v>
       </c>
       <c r="B70">
-        <v>13514.01775488513</v>
+        <v>14452.84995641878</v>
       </c>
       <c r="C70">
         <v>56224193.09222395</v>
       </c>
       <c r="D70">
-        <v>4419441.80799969</v>
+        <v>4419511.621852305</v>
       </c>
       <c r="E70">
-        <v>60657148.91797853</v>
+        <v>60658157.56403267</v>
       </c>
     </row>
     <row r="71">
@@ -1562,16 +1562,16 @@
         <v>2094</v>
       </c>
       <c r="B71">
-        <v>8042.537154707386</v>
+        <v>8480.090896353795</v>
       </c>
       <c r="C71">
         <v>43255256.65664101</v>
       </c>
       <c r="D71">
-        <v>3399860.763232355</v>
+        <v>3399893.300795916</v>
       </c>
       <c r="E71">
-        <v>46663159.95702807</v>
+        <v>46663630.04833327</v>
       </c>
     </row>
     <row r="72">
@@ -1579,16 +1579,16 @@
         <v>2095</v>
       </c>
       <c r="B72">
-        <v>4637.977553088474</v>
+        <v>4820.147928572237</v>
       </c>
       <c r="C72">
         <v>32901039.28271687</v>
       </c>
       <c r="D72">
-        <v>2585911.524827573</v>
+        <v>2585925.071461064</v>
       </c>
       <c r="E72">
-        <v>35491588.78509753</v>
+        <v>35491784.50210651</v>
       </c>
     </row>
     <row r="73">
@@ -1596,16 +1596,16 @@
         <v>2096</v>
       </c>
       <c r="B73">
-        <v>2587.021721890602</v>
+        <v>2652.979308297346</v>
       </c>
       <c r="C73">
         <v>24725121.58918776</v>
       </c>
       <c r="D73">
-        <v>1943245.759841227</v>
+        <v>1943250.664608243</v>
       </c>
       <c r="E73">
-        <v>26670954.37075087</v>
+        <v>26671025.2331043</v>
       </c>
     </row>
     <row r="74">
@@ -1613,16 +1613,16 @@
         <v>2097</v>
       </c>
       <c r="B74">
-        <v>1390.602981556135</v>
+        <v>1410.821339506151</v>
       </c>
       <c r="C74">
         <v>18340513.74324591</v>
       </c>
       <c r="D74">
-        <v>1441415.051710071</v>
+        <v>1441416.555196487</v>
       </c>
       <c r="E74">
-        <v>19783319.39793754</v>
+        <v>19783341.1197819</v>
       </c>
     </row>
     <row r="75">
@@ -1630,16 +1630,16 @@
         <v>2098</v>
       </c>
       <c r="B75">
-        <v>712.3450034435402</v>
+        <v>716.2562458103669</v>
       </c>
       <c r="C75">
         <v>13412501.00454104</v>
       </c>
       <c r="D75">
-        <v>1054090.846076513</v>
+        <v>1054091.136926036</v>
       </c>
       <c r="E75">
-        <v>14467304.19562099</v>
+        <v>14467308.39771288</v>
       </c>
     </row>
     <row r="76">
@@ -1647,16 +1647,16 @@
         <v>2099</v>
       </c>
       <c r="B76">
-        <v>346.8686951427341</v>
+        <v>347.5903795315784</v>
       </c>
       <c r="C76">
         <v>9657138.118848031</v>
       </c>
       <c r="D76">
-        <v>758943.9017221945</v>
+        <v>758943.9553884062</v>
       </c>
       <c r="E76">
-        <v>10416428.88926537</v>
+        <v>10416429.66461597</v>
       </c>
     </row>
     <row r="77">
@@ -1664,16 +1664,16 @@
         <v>2100</v>
       </c>
       <c r="B77">
-        <v>157.8802984902084</v>
+        <v>157.9615737741069</v>
       </c>
       <c r="C77">
         <v>6835156.920168932</v>
       </c>
       <c r="D77">
-        <v>537160.9832897456</v>
+        <v>537160.989333574</v>
       </c>
       <c r="E77">
-        <v>7372475.783757168</v>
+        <v>7372475.871076279</v>
       </c>
     </row>
     <row r="78">

</xml_diff>

<commit_message>
fix: est consideraba 300 peores
</commit_message>
<xml_diff>
--- a/res/egresos.xlsx
+++ b/res/egresos.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e64e3084cf54c9d/Documentos/Semestre 7/Pensiones/Proyecto/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_201BFED18F79A8D366075C52F37BD2720AC70CDD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F731872C-40C3-410B-A8E8-0E9916419311}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_60903FD08F79A8D366075C52F37BD2720A4BD97F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49BF5DA8-5AA1-4D49-86C4-B52943E64191}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -402,13 +389,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -433,16 +418,16 @@
         <v>2025</v>
       </c>
       <c r="B2">
-        <v>1880467976.676862</v>
+        <v>1875064470.3247409</v>
       </c>
       <c r="C2">
-        <v>147956668.69685829</v>
+        <v>273024684.85272998</v>
       </c>
       <c r="D2">
-        <v>143665929.49075419</v>
+        <v>141462564.25284281</v>
       </c>
       <c r="E2">
-        <v>2172090574.8644738</v>
+        <v>2289551719.4303141</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -450,16 +435,16 @@
         <v>2026</v>
       </c>
       <c r="B3">
-        <v>1775152818.5858481</v>
+        <v>1764732611.3479791</v>
       </c>
       <c r="C3">
-        <v>273066058.23066282</v>
+        <v>497199341.04982382</v>
       </c>
       <c r="D3">
-        <v>146163748.0048345</v>
+        <v>142142877.65777829</v>
       </c>
       <c r="E3">
-        <v>2194382624.8213449</v>
+        <v>2404074830.0555811</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -467,16 +452,16 @@
         <v>2027</v>
       </c>
       <c r="B4">
-        <v>1671639263.896055</v>
+        <v>1656591368.474839</v>
       </c>
       <c r="C4">
-        <v>438296516.24197072</v>
+        <v>775837193.26067078</v>
       </c>
       <c r="D4">
-        <v>151922292.47759891</v>
+        <v>146168230.77330899</v>
       </c>
       <c r="E4">
-        <v>2261858072.6156249</v>
+        <v>2578596792.5088191</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,16 +469,16 @@
         <v>2028</v>
       </c>
       <c r="B5">
-        <v>1574363313.820049</v>
+        <v>1554963587.0574341</v>
       </c>
       <c r="C5">
-        <v>683525971.35713923</v>
+        <v>1147089902.9605441</v>
       </c>
       <c r="D5">
-        <v>164406834.84166929</v>
+        <v>156982485.71952859</v>
       </c>
       <c r="E5">
-        <v>2422296120.018857</v>
+        <v>2859035975.7375059</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,16 +486,16 @@
         <v>2029</v>
       </c>
       <c r="B6">
-        <v>1486252351.9530439</v>
+        <v>1462868885.2175331</v>
       </c>
       <c r="C6">
-        <v>1010807382.464447</v>
+        <v>1525798925.3698151</v>
       </c>
       <c r="D6">
-        <v>183997827.6823239</v>
+        <v>175113842.71487769</v>
       </c>
       <c r="E6">
-        <v>2681057562.0998149</v>
+        <v>3163781653.3022261</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,16 +503,16 @@
         <v>2030</v>
       </c>
       <c r="B7">
-        <v>1396109940.869693</v>
+        <v>1369160247.033267</v>
       </c>
       <c r="C7">
-        <v>1279070370.5485411</v>
+        <v>1820613777.9863341</v>
       </c>
       <c r="D7">
-        <v>198777714.2222583</v>
+        <v>188565056.59482411</v>
       </c>
       <c r="E7">
-        <v>2873958025.640492</v>
+        <v>3378339081.6144252</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,16 +520,16 @@
         <v>2031</v>
       </c>
       <c r="B8">
-        <v>1313158516.9709511</v>
+        <v>1282903565.055856</v>
       </c>
       <c r="C8">
-        <v>1521114122.5109329</v>
+        <v>2214269483.2385778</v>
       </c>
       <c r="D8">
-        <v>212010877.59370929</v>
+        <v>200510226.36540321</v>
       </c>
       <c r="E8">
-        <v>3046283517.075593</v>
+        <v>3697683274.6598382</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,16 +537,16 @@
         <v>2032</v>
       </c>
       <c r="B9">
-        <v>1232941557.194804</v>
+        <v>1199594784.064779</v>
       </c>
       <c r="C9">
-        <v>1931554733.1732609</v>
+        <v>2540979080.456326</v>
       </c>
       <c r="D9">
-        <v>238661263.03734171</v>
+        <v>225958006.18789169</v>
       </c>
       <c r="E9">
-        <v>3403157553.405407</v>
+        <v>3966531870.7089958</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,16 +554,16 @@
         <v>2033</v>
       </c>
       <c r="B10">
-        <v>1153082999.692729</v>
+        <v>1117146585.3497331</v>
       </c>
       <c r="C10">
-        <v>2205242037.287127</v>
+        <v>2775828073.2979031</v>
       </c>
       <c r="D10">
-        <v>254572579.82982889</v>
+        <v>240732496.10213101</v>
       </c>
       <c r="E10">
-        <v>3612897616.8096852</v>
+        <v>4133707154.7497659</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,16 +571,16 @@
         <v>2034</v>
       </c>
       <c r="B11">
-        <v>1085736210.798929</v>
+        <v>1047352320.7850699</v>
       </c>
       <c r="C11">
-        <v>2512930025.2214098</v>
+        <v>3095257935.0111461</v>
       </c>
       <c r="D11">
-        <v>274068581.34330148</v>
+        <v>259046337.0454123</v>
       </c>
       <c r="E11">
-        <v>3872734817.3636408</v>
+        <v>4401656592.8416281</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,16 +588,16 @@
         <v>2035</v>
       </c>
       <c r="B12">
-        <v>1015662966.074368</v>
+        <v>975111042.19665504</v>
       </c>
       <c r="C12">
-        <v>2836802489.1948462</v>
+        <v>3406542587.8199492</v>
       </c>
       <c r="D12">
-        <v>294616749.01316971</v>
+        <v>278630545.48306942</v>
       </c>
       <c r="E12">
-        <v>4147082204.282383</v>
+        <v>4660284175.4996738</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,16 +605,16 @@
         <v>2036</v>
       </c>
       <c r="B13">
-        <v>950995473.63529754</v>
+        <v>908610399.51434541</v>
       </c>
       <c r="C13">
-        <v>3153691234.7616439</v>
+        <v>3680422146.8360929</v>
       </c>
       <c r="D13">
-        <v>315001833.61816013</v>
+        <v>297963155.00074452</v>
       </c>
       <c r="E13">
-        <v>4419688542.0151014</v>
+        <v>4886995701.3511839</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,16 +622,16 @@
         <v>2037</v>
       </c>
       <c r="B14">
-        <v>890378400.99063134</v>
+        <v>846465984.12709343</v>
       </c>
       <c r="C14">
-        <v>3463674136.8214531</v>
+        <v>3987617368.8154688</v>
       </c>
       <c r="D14">
-        <v>335129976.58366531</v>
+        <v>317054856.75896531</v>
       </c>
       <c r="E14">
-        <v>4689182514.3957491</v>
+        <v>5151138209.7015276</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -654,16 +639,16 @@
         <v>2038</v>
       </c>
       <c r="B15">
-        <v>831918878.25341904</v>
+        <v>786784130.46574128</v>
       </c>
       <c r="C15">
-        <v>3769626800.8199611</v>
+        <v>4249982907.8708401</v>
       </c>
       <c r="D15">
-        <v>355086893.78697342</v>
+        <v>336018528.61071831</v>
       </c>
       <c r="E15">
-        <v>4956632572.8603535</v>
+        <v>5372785566.9473</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -671,16 +656,16 @@
         <v>2039</v>
       </c>
       <c r="B16">
-        <v>778122743.88356733</v>
+        <v>732096322.34113419</v>
       </c>
       <c r="C16">
-        <v>4033448711.4929681</v>
+        <v>4427005240.5263929</v>
       </c>
       <c r="D16">
-        <v>372065575.12894058</v>
+        <v>352103573.25092173</v>
       </c>
       <c r="E16">
-        <v>5183637030.505476</v>
+        <v>5511205136.1184483</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,16 +673,16 @@
         <v>2040</v>
       </c>
       <c r="B17">
-        <v>725987916.2432363</v>
+        <v>679417834.48389888</v>
       </c>
       <c r="C17">
-        <v>4404170965.0362167</v>
+        <v>4700378000.384244</v>
       </c>
       <c r="D17">
-        <v>397555048.69700032</v>
+        <v>376712840.36626017</v>
       </c>
       <c r="E17">
-        <v>5527713929.9764538</v>
+        <v>5756508675.2344036</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,16 +690,16 @@
         <v>2041</v>
       </c>
       <c r="B18">
-        <v>675909485.54782426</v>
+        <v>629113315.07975876</v>
       </c>
       <c r="C18">
-        <v>4667115574.8737907</v>
+        <v>4947207926.8931046</v>
       </c>
       <c r="D18">
-        <v>414714336.37269872</v>
+        <v>392995119.49281669</v>
       </c>
       <c r="E18">
-        <v>5757739396.7943134</v>
+        <v>5969316361.4656801</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -722,16 +707,16 @@
         <v>2042</v>
       </c>
       <c r="B19">
-        <v>627617933.74288118</v>
+        <v>580912503.96303701</v>
       </c>
       <c r="C19">
-        <v>4891544067.5648518</v>
+        <v>5182069393.8398085</v>
       </c>
       <c r="D19">
-        <v>428966922.98355258</v>
+        <v>406441696.54067647</v>
       </c>
       <c r="E19">
-        <v>5948128924.2912865</v>
+        <v>6169423594.3435211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,16 +724,16 @@
         <v>2043</v>
       </c>
       <c r="B20">
-        <v>581585248.03027904</v>
+        <v>535339939.97448701</v>
       </c>
       <c r="C20">
-        <v>5143192292.5331345</v>
+        <v>5365394255.7475405</v>
       </c>
       <c r="D20">
-        <v>445514223.40138203</v>
+        <v>422237550.01942742</v>
       </c>
       <c r="E20">
-        <v>6170291763.9647951</v>
+        <v>6322971745.7414541</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -756,16 +741,16 @@
         <v>2044</v>
       </c>
       <c r="B21">
-        <v>537284885.89400613</v>
+        <v>491784441.3606832</v>
       </c>
       <c r="C21">
-        <v>5495846568.5523624</v>
+        <v>5680197937.1307716</v>
       </c>
       <c r="D21">
-        <v>470116041.59142393</v>
+        <v>446133012.40665472</v>
       </c>
       <c r="E21">
-        <v>6503247496.0377922</v>
+        <v>6618115390.8981094</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,16 +758,16 @@
         <v>2045</v>
       </c>
       <c r="B22">
-        <v>494651983.24945062</v>
+        <v>450213033.30866992</v>
       </c>
       <c r="C22">
-        <v>5820090731.1171837</v>
+        <v>5917852971.6784496</v>
       </c>
       <c r="D22">
-        <v>492597595.95097041</v>
+        <v>467985064.90809208</v>
       </c>
       <c r="E22">
-        <v>6807340310.317605</v>
+        <v>6836051069.8952122</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,16 +775,16 @@
         <v>2046</v>
       </c>
       <c r="B23">
-        <v>453684530.28326768</v>
+        <v>410613700.70397413</v>
       </c>
       <c r="C23">
-        <v>6089648915.1665096</v>
+        <v>6080701651.1342382</v>
       </c>
       <c r="D23">
-        <v>510894020.656322</v>
+        <v>485715141.58324963</v>
       </c>
       <c r="E23">
-        <v>7054227466.1061001</v>
+        <v>6977030493.4214621</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -807,16 +792,16 @@
         <v>2047</v>
       </c>
       <c r="B24">
-        <v>414381308.29013819</v>
+        <v>372959422.56024587</v>
       </c>
       <c r="C24">
-        <v>6318139849.3001661</v>
+        <v>6212220206.4108133</v>
       </c>
       <c r="D24">
-        <v>526075774.38953</v>
+        <v>500416140.29246378</v>
       </c>
       <c r="E24">
-        <v>7258596931.9798346</v>
+        <v>7085595769.2635231</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,16 +809,16 @@
         <v>2048</v>
       </c>
       <c r="B25">
-        <v>376724769.73687118</v>
+        <v>337215274.18982953</v>
       </c>
       <c r="C25">
-        <v>6521743440.9019051</v>
+        <v>6299364322.788866</v>
       </c>
       <c r="D25">
-        <v>539413429.77527738</v>
+        <v>513350145.80405009</v>
       </c>
       <c r="E25">
-        <v>7437881640.4140539</v>
+        <v>7149929742.7827463</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -841,16 +826,16 @@
         <v>2049</v>
       </c>
       <c r="B26">
-        <v>340737916.91279358</v>
+        <v>303376935.71308851</v>
       </c>
       <c r="C26">
-        <v>6582451142.0336952</v>
+        <v>6347749984.2452288</v>
       </c>
       <c r="D26">
-        <v>541635142.81790316</v>
+        <v>515260683.38966322</v>
       </c>
       <c r="E26">
-        <v>7464824201.7643919</v>
+        <v>7166387603.3479795</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -858,16 +843,16 @@
         <v>2050</v>
       </c>
       <c r="B27">
-        <v>306461849.32079911</v>
+        <v>271452610.35055411</v>
       </c>
       <c r="C27">
-        <v>6668801554.0211182</v>
+        <v>6397731534.6682615</v>
       </c>
       <c r="D27">
-        <v>545989093.24248207</v>
+        <v>519371032.48157543</v>
       </c>
       <c r="E27">
-        <v>7521252496.5843992</v>
+        <v>7188555177.500392</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -875,16 +860,16 @@
         <v>2051</v>
       </c>
       <c r="B28">
-        <v>273948733.21102703</v>
+        <v>241458065.20978051</v>
       </c>
       <c r="C28">
-        <v>6690687000.5457764</v>
+        <v>6296230510.1168842</v>
       </c>
       <c r="D28">
-        <v>545398232.92819476</v>
+        <v>518623684.97951972</v>
       </c>
       <c r="E28">
-        <v>7510033966.6849995</v>
+        <v>7056312260.3061848</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,16 +877,16 @@
         <v>2052</v>
       </c>
       <c r="B29">
-        <v>243265697.95057061</v>
+        <v>213419229.50000361</v>
       </c>
       <c r="C29">
-        <v>6663102818.6745892</v>
+        <v>6193771509.4332991</v>
       </c>
       <c r="D29">
-        <v>541046258.78792369</v>
+        <v>514199782.07821202</v>
       </c>
       <c r="E29">
-        <v>7447414775.4130831</v>
+        <v>6921390521.0115147</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,16 +894,16 @@
         <v>2053</v>
       </c>
       <c r="B30">
-        <v>214478735.38033399</v>
+        <v>187356017.14784089</v>
       </c>
       <c r="C30">
-        <v>6540030476.5348997</v>
+        <v>6056950094.132823</v>
       </c>
       <c r="D30">
-        <v>529322000.80372232</v>
+        <v>502490499.25048631</v>
       </c>
       <c r="E30">
-        <v>7283831212.718956</v>
+        <v>6746796610.5311499</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,16 +911,16 @@
         <v>2054</v>
       </c>
       <c r="B31">
-        <v>187652812.0972563</v>
+        <v>163284504.2168144</v>
       </c>
       <c r="C31">
-        <v>6386691959.1716547</v>
+        <v>5911127866.0218678</v>
       </c>
       <c r="D31">
-        <v>515356258.71158773</v>
+        <v>488626881.06197572</v>
       </c>
       <c r="E31">
-        <v>7089701029.9804993</v>
+        <v>6563039251.3006573</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,16 +928,16 @@
         <v>2055</v>
       </c>
       <c r="B32">
-        <v>162858495.40331909</v>
+        <v>141224866.18251839</v>
       </c>
       <c r="C32">
-        <v>6200995099.0908394</v>
+        <v>5721845884.5616379</v>
       </c>
       <c r="D32">
-        <v>498990255.51749128</v>
+        <v>472439181.80986679</v>
       </c>
       <c r="E32">
-        <v>6862843850.0116501</v>
+        <v>6335509932.5540228</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,16 +945,16 @@
         <v>2056</v>
       </c>
       <c r="B33">
-        <v>140162378.3742007</v>
+        <v>121193652.3915122</v>
       </c>
       <c r="C33">
-        <v>5963985960.5997372</v>
+        <v>5482965633.305419</v>
       </c>
       <c r="D33">
-        <v>478739823.11448538</v>
+        <v>452450213.64629883</v>
       </c>
       <c r="E33">
-        <v>6582888162.0884237</v>
+        <v>6056609499.3432293</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,16 +962,16 @@
         <v>2057</v>
       </c>
       <c r="B34">
-        <v>119599554.34552699</v>
+        <v>103179586.957252</v>
       </c>
       <c r="C34">
-        <v>5701901190.0834227</v>
+        <v>5244279418.5521984</v>
       </c>
       <c r="D34">
-        <v>456669901.90009809</v>
+        <v>430717603.16950673</v>
       </c>
       <c r="E34">
-        <v>6278170646.3290472</v>
+        <v>5778176608.678957</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,16 +979,16 @@
         <v>2058</v>
       </c>
       <c r="B35">
-        <v>101175172.4034119</v>
+        <v>87146791.089476481</v>
       </c>
       <c r="C35">
-        <v>5428627332.4453001</v>
+        <v>4981733204.3188868</v>
       </c>
       <c r="D35">
-        <v>433872703.14252579</v>
+        <v>408326980.70833111</v>
       </c>
       <c r="E35">
-        <v>5963675207.9912376</v>
+        <v>5477206976.1166945</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,16 +996,16 @@
         <v>2059</v>
       </c>
       <c r="B36">
-        <v>84871191.678459823</v>
+        <v>73042001.80689466</v>
       </c>
       <c r="C36">
-        <v>5156752872.5686092</v>
+        <v>4722044288.8066959</v>
       </c>
       <c r="D36">
-        <v>411336716.06359881</v>
+        <v>386258407.45599627</v>
       </c>
       <c r="E36">
-        <v>5652960780.310668</v>
+        <v>5181344698.0695868</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,16 +1013,16 @@
         <v>2060</v>
       </c>
       <c r="B37">
-        <v>70636890.228472278</v>
+        <v>60787925.899342127</v>
       </c>
       <c r="C37">
-        <v>4866878298.6880684</v>
+        <v>4445827039.1752167</v>
       </c>
       <c r="D37">
-        <v>387534202.37443292</v>
+        <v>362982577.05473399</v>
       </c>
       <c r="E37">
-        <v>5325049391.2909737</v>
+        <v>4869597542.1292934</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,16 +1030,16 @@
         <v>2061</v>
       </c>
       <c r="B38">
-        <v>58381900.22765249</v>
+        <v>50278812.433501117</v>
       </c>
       <c r="C38">
-        <v>4575106060.8402119</v>
+        <v>4173666906.673368</v>
       </c>
       <c r="D38">
-        <v>363724453.16424233</v>
+        <v>339756641.93762797</v>
       </c>
       <c r="E38">
-        <v>4997212414.2321072</v>
+        <v>4563702361.0444965</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,16 +1047,16 @@
         <v>2062</v>
       </c>
       <c r="B39">
-        <v>47978599.243895032</v>
+        <v>41382571.273546956</v>
       </c>
       <c r="C39">
-        <v>4289646418.5876312</v>
+        <v>3906753209.805963</v>
       </c>
       <c r="D39">
-        <v>340543771.23551178</v>
+        <v>317208768.60380572</v>
       </c>
       <c r="E39">
-        <v>4678168789.0670376</v>
+        <v>4265344549.6833162</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,16 +1064,16 @@
         <v>2063</v>
       </c>
       <c r="B40">
-        <v>39267920.671728298</v>
+        <v>33945194.73889415</v>
       </c>
       <c r="C40">
-        <v>4009845592.7412548</v>
+        <v>3642298584.3753762</v>
       </c>
       <c r="D40">
-        <v>317929532.08097351</v>
+        <v>295270346.99934667</v>
       </c>
       <c r="E40">
-        <v>4367043045.4939566</v>
+        <v>3971514126.113616</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,16 +1081,16 @@
         <v>2064</v>
       </c>
       <c r="B41">
-        <v>32062918.385136861</v>
+        <v>27794318.761961222</v>
       </c>
       <c r="C41">
-        <v>3729979177.9348722</v>
+        <v>3389364415.4506078</v>
       </c>
       <c r="D41">
-        <v>295418557.38477182</v>
+        <v>273476201.08168209</v>
       </c>
       <c r="E41">
-        <v>4057460653.7047811</v>
+        <v>3690634935.294251</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1113,16 +1098,16 @@
         <v>2065</v>
       </c>
       <c r="B42">
-        <v>26170788.963886488</v>
+        <v>22758324.692854811</v>
       </c>
       <c r="C42">
-        <v>3455256974.278594</v>
+        <v>3137402962.9047298</v>
       </c>
       <c r="D42">
-        <v>273406426.90989703</v>
+        <v>252220237.22631091</v>
       </c>
       <c r="E42">
-        <v>3754834190.1523771</v>
+        <v>3412381524.823895</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,16 +1115,16 @@
         <v>2066</v>
       </c>
       <c r="B43">
-        <v>21393716.561288819</v>
+        <v>18665328.684356909</v>
       </c>
       <c r="C43">
-        <v>3197104658.60184</v>
+        <v>2895785980.631938</v>
       </c>
       <c r="D43">
-        <v>252776800.88078669</v>
+        <v>232380717.58524209</v>
       </c>
       <c r="E43">
-        <v>3471275176.0439148</v>
+        <v>3146832026.9015369</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,16 +1132,16 @@
         <v>2067</v>
       </c>
       <c r="B44">
-        <v>17539967.580567759</v>
+        <v>15351621.152417749</v>
       </c>
       <c r="C44">
-        <v>2947974373.0439429</v>
+        <v>2666168254.1701331</v>
       </c>
       <c r="D44">
-        <v>232922687.72492579</v>
+        <v>213348809.2903595</v>
       </c>
       <c r="E44">
-        <v>3198437028.3494372</v>
+        <v>2894868684.6129098</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,16 +1149,16 @@
         <v>2068</v>
       </c>
       <c r="B45">
-        <v>14434607.181646699</v>
+        <v>12669520.57881755</v>
       </c>
       <c r="C45">
-        <v>2707433167.6729908</v>
+        <v>2445897343.7148242</v>
       </c>
       <c r="D45">
-        <v>213797420.07595921</v>
+        <v>195075249.1387521</v>
       </c>
       <c r="E45">
-        <v>2935665194.9305968</v>
+        <v>2653642113.432394</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,16 +1166,16 @@
         <v>2069</v>
       </c>
       <c r="B46">
-        <v>11926109.493350949</v>
+        <v>10492127.392676281</v>
       </c>
       <c r="C46">
-        <v>2477144500.3878469</v>
+        <v>2236978796.6671839</v>
       </c>
       <c r="D46">
-        <v>195520765.53922379</v>
+        <v>177677382.83587179</v>
       </c>
       <c r="E46">
-        <v>2684591375.4204221</v>
+        <v>2425148306.8957319</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,16 +1183,16 @@
         <v>2070</v>
       </c>
       <c r="B47">
-        <v>9888793.7847502232</v>
+        <v>8714773.4957074188</v>
       </c>
       <c r="C47">
-        <v>2259461632.950758</v>
+        <v>2039884675.236114</v>
       </c>
       <c r="D47">
-        <v>178268567.2633146</v>
+        <v>161328082.3392722</v>
       </c>
       <c r="E47">
-        <v>2447618993.9988232</v>
+        <v>2209927531.071094</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,16 +1200,16 @@
         <v>2071</v>
       </c>
       <c r="B48">
-        <v>8221547.6230545864</v>
+        <v>7253373.5581587721</v>
       </c>
       <c r="C48">
-        <v>2054287083.0999961</v>
+        <v>1854411576.4980831</v>
       </c>
       <c r="D48">
-        <v>162025854.24651501</v>
+        <v>146009114.69860169</v>
       </c>
       <c r="E48">
-        <v>2224534484.9695649</v>
+        <v>2007674064.754843</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,16 +1217,16 @@
         <v>2072</v>
       </c>
       <c r="B49">
-        <v>6845666.4305333504</v>
+        <v>6042432.6929495912</v>
       </c>
       <c r="C49">
-        <v>1861205626.894347</v>
+        <v>1680160976.886025</v>
       </c>
       <c r="D49">
-        <v>146754314.72949839</v>
+        <v>131678864.4047624</v>
       </c>
       <c r="E49">
-        <v>2014805608.054379</v>
+        <v>1817882273.983737</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,16 +1234,16 @@
         <v>2073</v>
       </c>
       <c r="B50">
-        <v>5701040.5228371788</v>
+        <v>5031742.4097335935</v>
       </c>
       <c r="C50">
-        <v>1679815637.0940981</v>
+        <v>1516737557.842576</v>
       </c>
       <c r="D50">
-        <v>132418057.2824861</v>
+        <v>118297442.20769</v>
       </c>
       <c r="E50">
-        <v>1817934734.899421</v>
+        <v>1640066742.4599991</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,16 +1251,16 @@
         <v>2074</v>
       </c>
       <c r="B51">
-        <v>4742338.3304144274</v>
+        <v>4183219.59936509</v>
       </c>
       <c r="C51">
-        <v>1509803548.545943</v>
+        <v>1363814232.6976359</v>
       </c>
       <c r="D51">
-        <v>118989183.3789776</v>
+        <v>105832309.32765</v>
       </c>
       <c r="E51">
-        <v>1633535070.2553351</v>
+        <v>1473829761.624651</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,16 +1268,16 @@
         <v>2075</v>
       </c>
       <c r="B52">
-        <v>3935312.034524159</v>
+        <v>3467929.0914756618</v>
       </c>
       <c r="C52">
-        <v>1350941625.2736559</v>
+        <v>1221119322.0808439</v>
       </c>
       <c r="D52">
-        <v>106447341.7200627</v>
+        <v>94257476.307642817</v>
       </c>
       <c r="E52">
-        <v>1461324279.0282431</v>
+        <v>1318844727.4799631</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,16 +1285,16 @@
         <v>2076</v>
       </c>
       <c r="B53">
-        <v>3253456.6847214098</v>
+        <v>2863315.3700107788</v>
       </c>
       <c r="C53">
-        <v>1202966748.352674</v>
+        <v>1088367967.7254951</v>
       </c>
       <c r="D53">
-        <v>94769959.736714229</v>
+        <v>83544417.677061319</v>
       </c>
       <c r="E53">
-        <v>1300990164.7741101</v>
+        <v>1174775700.772567</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,16 +1302,16 @@
         <v>2077</v>
       </c>
       <c r="B54">
-        <v>2675864.3640524568</v>
+        <v>2351411.6868636529</v>
       </c>
       <c r="C54">
-        <v>1065602028.686601</v>
+        <v>965259697.15346622</v>
       </c>
       <c r="D54">
-        <v>83933786.896617264</v>
+        <v>73663318.312148735</v>
       </c>
       <c r="E54">
-        <v>1152211679.9472711</v>
+        <v>1041274427.1524791</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,16 +1319,16 @@
         <v>2078</v>
       </c>
       <c r="B55">
-        <v>2185887.61838073</v>
+        <v>1917768.5746119269</v>
       </c>
       <c r="C55">
-        <v>938594769.84761715</v>
+        <v>851512163.85427201</v>
       </c>
       <c r="D55">
-        <v>73917780.696711913</v>
+        <v>64586149.380949043</v>
       </c>
       <c r="E55">
-        <v>1014698438.16271</v>
+        <v>918016081.80983293</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,16 +1336,16 @@
         <v>2079</v>
       </c>
       <c r="B56">
-        <v>1770392.4195152</v>
+        <v>1550848.761228028</v>
       </c>
       <c r="C56">
-        <v>821747504.15246606</v>
+        <v>746889196.55397856</v>
       </c>
       <c r="D56">
-        <v>64705491.309361093</v>
+        <v>56289058.617527381</v>
       </c>
       <c r="E56">
-        <v>888223387.88134241</v>
+        <v>804729103.93273401</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,16 +1353,16 @@
         <v>2080</v>
       </c>
       <c r="B57">
-        <v>1419019.702575519</v>
+        <v>1241422.5921559981</v>
       </c>
       <c r="C57">
-        <v>714864325.99838126</v>
+        <v>651164700.91972446</v>
       </c>
       <c r="D57">
-        <v>56280790.519181572</v>
+        <v>48748433.916902438</v>
       </c>
       <c r="E57">
-        <v>772564136.22013843</v>
+        <v>701154557.42878294</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,16 +1370,16 @@
         <v>2081</v>
       </c>
       <c r="B58">
-        <v>1123389.9167595119</v>
+        <v>981910.59325146268</v>
       </c>
       <c r="C58">
-        <v>617690250.99053812</v>
+        <v>564072895.85054076</v>
       </c>
       <c r="D58">
-        <v>48623048.964537069</v>
+        <v>41936524.030783869</v>
       </c>
       <c r="E58">
-        <v>667436689.87183464</v>
+        <v>606991330.47457612</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1402,16 +1387,16 @@
         <v>2082</v>
       </c>
       <c r="B59">
-        <v>876625.39895824308</v>
+        <v>765986.98358147347</v>
       </c>
       <c r="C59">
-        <v>529920945.86897922</v>
+        <v>485308300.61785781</v>
       </c>
       <c r="D59">
-        <v>41707866.834781677</v>
+        <v>35822392.625649028</v>
       </c>
       <c r="E59">
-        <v>572505438.10271907</v>
+        <v>521896680.22708827</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,16 +1404,16 @@
         <v>2083</v>
       </c>
       <c r="B60">
-        <v>672963.95120702125</v>
+        <v>588286.62890181597</v>
       </c>
       <c r="C60">
-        <v>451211201.73532248</v>
+        <v>414542976.83493578</v>
       </c>
       <c r="D60">
-        <v>35507711.774761043</v>
+        <v>30372898.042151231</v>
       </c>
       <c r="E60">
-        <v>487391877.46129048</v>
+        <v>445504161.50598878</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,16 +1421,16 @@
         <v>2084</v>
       </c>
       <c r="B61">
-        <v>507361.53457391239</v>
+        <v>444106.9935460061</v>
       </c>
       <c r="C61">
-        <v>381191203.61317438</v>
+        <v>351438223.16393149</v>
       </c>
       <c r="D61">
-        <v>29993168.39111368</v>
+        <v>25553899.372556109</v>
       </c>
       <c r="E61">
-        <v>411691733.53886199</v>
+        <v>377436229.53003359</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,16 +1438,16 @@
         <v>2085</v>
       </c>
       <c r="B62">
-        <v>375146.44055656838</v>
+        <v>329133.92652942613</v>
       </c>
       <c r="C62">
-        <v>319445939.31298429</v>
+        <v>295623584.48005968</v>
       </c>
       <c r="D62">
-        <v>25131294.79220422</v>
+        <v>21328872.362181779</v>
       </c>
       <c r="E62">
-        <v>344952380.54574507</v>
+        <v>317281590.76877087</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,16 +1455,16 @@
         <v>2086</v>
       </c>
       <c r="B63">
-        <v>271737.65178317571</v>
+        <v>239215.55119182781</v>
       </c>
       <c r="C63">
-        <v>265481056.5849613</v>
+        <v>246671762.50970861</v>
       </c>
       <c r="D63">
-        <v>20882918.83855268</v>
+        <v>17656703.452076819</v>
       </c>
       <c r="E63">
-        <v>286635713.07529712</v>
+        <v>264567681.5129773</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,16 +1472,16 @@
         <v>2087</v>
       </c>
       <c r="B64">
-        <v>192623.7383773833</v>
+        <v>170338.34205522531</v>
       </c>
       <c r="C64">
-        <v>218737412.4829796</v>
+        <v>204106043.6672723</v>
       </c>
       <c r="D64">
-        <v>17203780.02700324</v>
+        <v>14492813.270346491</v>
       </c>
       <c r="E64">
-        <v>236133816.24836019</v>
+        <v>218769195.27967411</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,16 +1489,16 @@
         <v>2088</v>
       </c>
       <c r="B65">
-        <v>133475.12496542299</v>
+        <v>118711.25504947281</v>
       </c>
       <c r="C65">
-        <v>178621698.46566331</v>
+        <v>167422303.18664649</v>
       </c>
       <c r="D65">
-        <v>14046944.348704901</v>
+        <v>11791321.99200912</v>
       </c>
       <c r="E65">
-        <v>192802117.93933359</v>
+        <v>179332336.43370509</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,16 +1506,16 @@
         <v>2089</v>
       </c>
       <c r="B66">
-        <v>90306.522440687302</v>
+        <v>80883.488171971912</v>
       </c>
       <c r="C66">
-        <v>144531300.05362809</v>
+        <v>136107293.5088248</v>
       </c>
       <c r="D66">
-        <v>11364769.851882599</v>
+        <v>9506714.1254327372</v>
       </c>
       <c r="E66">
-        <v>155986376.4279514</v>
+        <v>145694891.12242949</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,16 +1523,16 @@
         <v>2090</v>
       </c>
       <c r="B67">
-        <v>59579.331680910407</v>
+        <v>53813.392919712307</v>
       </c>
       <c r="C67">
-        <v>115854981.571022</v>
+        <v>109638412.610193</v>
       </c>
       <c r="D67">
-        <v>9108968.0751725882</v>
+        <v>7593818.1605135929</v>
       </c>
       <c r="E67">
-        <v>125023528.9778755</v>
+        <v>117286044.1636263</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,16 +1540,16 @@
         <v>2091</v>
       </c>
       <c r="B68">
-        <v>38262.169886319833</v>
+        <v>34905.00498658049</v>
       </c>
       <c r="C68">
-        <v>91975629.301864237</v>
+        <v>87486071.981144235</v>
       </c>
       <c r="D68">
-        <v>7230824.3040454267</v>
+        <v>6007922.0087512974</v>
       </c>
       <c r="E68">
-        <v>99244715.775795981</v>
+        <v>93528898.994882122</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,16 +1557,16 @@
         <v>2092</v>
       </c>
       <c r="B69">
-        <v>23875.580123899359</v>
+        <v>22034.1725601988</v>
       </c>
       <c r="C69">
-        <v>72289011.787892997</v>
+        <v>69128349.747029021</v>
       </c>
       <c r="D69">
-        <v>5682675.4518618807</v>
+        <v>4705960.2680958109</v>
       </c>
       <c r="E69">
-        <v>77995562.819878787</v>
+        <v>73856344.187685028</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,16 +1574,16 @@
         <v>2093</v>
       </c>
       <c r="B70">
-        <v>14452.84995641878</v>
+        <v>13514.01775488513</v>
       </c>
       <c r="C70">
-        <v>56224193.09222395</v>
+        <v>54068155.5365052</v>
       </c>
       <c r="D70">
-        <v>4419511.6218523048</v>
+        <v>3647783.9710556678</v>
       </c>
       <c r="E70">
-        <v>60658157.564032666</v>
+        <v>57729453.525315747</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,16 +1591,16 @@
         <v>2094</v>
       </c>
       <c r="B71">
-        <v>8480.090896353795</v>
+        <v>8042.5371547073864</v>
       </c>
       <c r="C71">
-        <v>43255256.656641006</v>
+        <v>41843615.996626116</v>
       </c>
       <c r="D71">
-        <v>3399893.300795916</v>
+        <v>2796830.2228980851</v>
       </c>
       <c r="E71">
-        <v>46663630.048333272</v>
+        <v>44648488.756678917</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,16 +1608,16 @@
         <v>2095</v>
       </c>
       <c r="B72">
-        <v>4820.1479285722371</v>
+        <v>4637.9775530884745</v>
       </c>
       <c r="C72">
-        <v>32901039.28271687</v>
+        <v>32028703.88932246</v>
       </c>
       <c r="D72">
-        <v>2585925.0714610638</v>
+        <v>2119997.774211328</v>
       </c>
       <c r="E72">
-        <v>35491784.50210651</v>
+        <v>34153339.641086876</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1640,16 +1625,16 @@
         <v>2096</v>
       </c>
       <c r="B73">
-        <v>2652.9793082973461</v>
+        <v>2587.0217218906018</v>
       </c>
       <c r="C73">
-        <v>24725121.58918776</v>
+        <v>24233775.23544376</v>
       </c>
       <c r="D73">
-        <v>1943250.6646082429</v>
+        <v>1587547.7941147459</v>
       </c>
       <c r="E73">
-        <v>26671025.2331043</v>
+        <v>25823910.051280402</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,16 +1642,16 @@
         <v>2097</v>
       </c>
       <c r="B74">
-        <v>1410.8213395061509</v>
+        <v>1390.6029815561351</v>
       </c>
       <c r="C74">
-        <v>18340513.743245911</v>
+        <v>18110178.806836382</v>
       </c>
       <c r="D74">
-        <v>1441416.5551964871</v>
+        <v>1173318.269283463</v>
       </c>
       <c r="E74">
-        <v>19783341.1197819</v>
+        <v>19284887.6791014</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,16 +1659,16 @@
         <v>2098</v>
       </c>
       <c r="B75">
-        <v>716.25624581036686</v>
+        <v>712.34500344354024</v>
       </c>
       <c r="C75">
-        <v>13412501.004541039</v>
+        <v>13353463.622441599</v>
       </c>
       <c r="D75">
-        <v>1054091.1369260361</v>
+        <v>854825.32232445513</v>
       </c>
       <c r="E75">
-        <v>14467308.397712881</v>
+        <v>14209001.2897695</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,16 +1676,16 @@
         <v>2099</v>
       </c>
       <c r="B76">
-        <v>347.59037953157838</v>
+        <v>346.86869514273411</v>
       </c>
       <c r="C76">
-        <v>9657138.1188480314</v>
+        <v>9703189.5537421703</v>
       </c>
       <c r="D76">
-        <v>758943.95538840618</v>
+        <v>613091.79540732375</v>
       </c>
       <c r="E76">
-        <v>10416429.66461597</v>
+        <v>10316628.217844641</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,16 +1693,16 @@
         <v>2100</v>
       </c>
       <c r="B77">
-        <v>157.96157377410691</v>
+        <v>157.88029849020839</v>
       </c>
       <c r="C77">
-        <v>6835156.9201689316</v>
+        <v>6938336.3271142328</v>
       </c>
       <c r="D77">
-        <v>537160.98933357396</v>
+        <v>432198.95941688248</v>
       </c>
       <c r="E77">
-        <v>7372475.8710762793</v>
+        <v>7370693.1668296056</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,13 +1713,13 @@
         <v>66.353648233608112</v>
       </c>
       <c r="C78">
-        <v>4746753.7381171882</v>
+        <v>4873832.5439235559</v>
       </c>
       <c r="D78">
-        <v>373034.43684100878</v>
+        <v>298910.15364468843</v>
       </c>
       <c r="E78">
-        <v>5119854.5286064306</v>
+        <v>5172809.0512164785</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,13 +1730,13 @@
         <v>25.519258063129751</v>
       </c>
       <c r="C79">
-        <v>3227081.047569768</v>
+        <v>3356206.07137352</v>
       </c>
       <c r="D79">
-        <v>253606.04595749811</v>
+        <v>202354.38615965919</v>
       </c>
       <c r="E79">
-        <v>3480712.6127853291</v>
+        <v>3558585.9767912431</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,13 +1747,13 @@
         <v>8.8997611911991221</v>
       </c>
       <c r="C80">
-        <v>2142156.8862361922</v>
+        <v>2260131.2915352639</v>
       </c>
       <c r="D80">
-        <v>168344.7054234898</v>
+        <v>133739.64633015401</v>
       </c>
       <c r="E80">
-        <v>2310510.491420873</v>
+        <v>2393879.837626609</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1779,13 +1764,13 @@
         <v>2.79419650510133</v>
       </c>
       <c r="C81">
-        <v>1384406.78230867</v>
+        <v>1484395.995983154</v>
       </c>
       <c r="D81">
-        <v>108795.5239620482</v>
+        <v>86043.683114612533</v>
       </c>
       <c r="E81">
-        <v>1493205.1004672239</v>
+        <v>1570442.4732942721</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1796,13 +1781,13 @@
         <v>0.77815415869931659</v>
       </c>
       <c r="C82">
-        <v>868189.8671750729</v>
+        <v>947892.69634570309</v>
       </c>
       <c r="D82">
-        <v>68227.830446134642</v>
+        <v>53709.097233808418</v>
       </c>
       <c r="E82">
-        <v>936418.4757753663</v>
+        <v>1001602.57173367</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,13 +1798,13 @@
         <v>0.17630973068167119</v>
       </c>
       <c r="C83">
-        <v>526247.8793532108</v>
+        <v>586364.4109393541</v>
       </c>
       <c r="D83">
-        <v>41355.852416353031</v>
+        <v>32398.33886368425</v>
       </c>
       <c r="E83">
-        <v>567603.90807929449</v>
+        <v>618762.92611276894</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,13 +1815,13 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>306845.0392185924</v>
+        <v>349801.90347028471</v>
       </c>
       <c r="D84">
-        <v>24113.796238419291</v>
+        <v>18795.786014294681</v>
       </c>
       <c r="E84">
-        <v>330958.83545701171</v>
+        <v>368597.68948457937</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,13 +1832,13 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <v>171139.0680471895</v>
+        <v>200155.82394886229</v>
       </c>
       <c r="D85">
-        <v>13449.17495108342</v>
+        <v>10428.04368764939</v>
       </c>
       <c r="E85">
-        <v>184588.24299827291</v>
+        <v>210583.86763651171</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,13 +1849,13 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <v>90722.978070201207</v>
+        <v>109158.9761598325</v>
       </c>
       <c r="D86">
-        <v>7129.577238395379</v>
+        <v>5497.6119644899654</v>
       </c>
       <c r="E86">
-        <v>97852.55530859658</v>
+        <v>114656.5881243225</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1881,13 +1866,13 @@
         <v>0</v>
       </c>
       <c r="C87">
-        <v>45388.574638803453</v>
+        <v>56332.939146573888</v>
       </c>
       <c r="D87">
-        <v>3566.9171748046119</v>
+        <v>2734.589907951985</v>
       </c>
       <c r="E87">
-        <v>48955.491813608067</v>
+        <v>59067.529054525883</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,13 +1883,13 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>21257.439269302311</v>
+        <v>27261.044834391261</v>
       </c>
       <c r="D88">
-        <v>1670.542109450108</v>
+        <v>1272.9494191318779</v>
       </c>
       <c r="E88">
-        <v>22927.981378752411</v>
+        <v>28533.994253523138</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,13 +1900,13 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>9235.054872820243</v>
+        <v>12235.68768846608</v>
       </c>
       <c r="D89">
-        <v>725.74818879560075</v>
+        <v>549.46577723410019</v>
       </c>
       <c r="E89">
-        <v>9960.803061615843</v>
+        <v>12785.153465700179</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1932,13 +1917,13 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>3686.734622954204</v>
+        <v>5031.5164956090948</v>
       </c>
       <c r="D90">
-        <v>289.72659199391921</v>
+        <v>217.83481838858631</v>
       </c>
       <c r="E90">
-        <v>3976.4612149481241</v>
+        <v>5249.3513139976812</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1949,13 +1934,13 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <v>1342.9849469771709</v>
+        <v>1877.180708975937</v>
       </c>
       <c r="D91">
-        <v>105.54013010978341</v>
+        <v>78.732910104246031</v>
       </c>
       <c r="E91">
-        <v>1448.5250770869541</v>
+        <v>1955.913619080183</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,13 +1951,13 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>440.04033291327028</v>
+        <v>623.23044328852268</v>
       </c>
       <c r="D92">
-        <v>34.581112836559903</v>
+        <v>25.58194999413757</v>
       </c>
       <c r="E92">
-        <v>474.62144574983017</v>
+        <v>648.8123932826602</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -1983,13 +1968,13 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>122.6821477151809</v>
+        <v>169.3044964436524</v>
       </c>
       <c r="D93">
-        <v>9.6411280417932765</v>
+        <v>7.0650618274492478</v>
       </c>
       <c r="E93">
-        <v>132.3232757569742</v>
+        <v>176.36955827110171</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2000,13 +1985,13 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <v>28.525826629333292</v>
+        <v>35.804912239841059</v>
       </c>
       <c r="D94">
-        <v>2.2417373037019872</v>
+        <v>1.617431215271647</v>
       </c>
       <c r="E94">
-        <v>30.76756393303528</v>
+        <v>37.422343455112703</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2017,13 +2002,13 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <v>6.1591197991529372</v>
+        <v>7.1129140062323506</v>
       </c>
       <c r="D95">
-        <v>0.48402203347659262</v>
+        <v>0.34298691981136642</v>
       </c>
       <c r="E95">
-        <v>6.6431418326295297</v>
+        <v>7.455900926043717</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>